<commit_message>
Changed lat and long values in the file
</commit_message>
<xml_diff>
--- a/data/UK_Regions.xlsx
+++ b/data/UK_Regions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TejasKundu\PycharmProjects\Geo_visuals\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4203206B-28B0-4A28-B18E-16FF4E148E2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE81109-E7CE-4AF0-B9C6-7BC8559B81EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C0D29889-3A2F-4756-82E4-31BB4CE383CE}"/>
   </bookViews>
@@ -504,7 +504,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,10 +532,10 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>51.451019000000002</v>
+        <v>51.033999100000003</v>
       </c>
       <c r="C2">
-        <v>-0.99349100000000001</v>
+        <v>-2.9490119160211901</v>
       </c>
       <c r="D2">
         <v>20</v>
@@ -546,10 +546,10 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>51.500152</v>
+        <v>51.50002095</v>
       </c>
       <c r="C3">
-        <v>-0.12623599999999999</v>
+        <v>-0.19244203566212201</v>
       </c>
       <c r="D3">
         <v>30</v>
@@ -560,10 +560,10 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>51.449579999999997</v>
+        <v>51.451019099999897</v>
       </c>
       <c r="C4">
-        <v>-2.5937079999999999</v>
+        <v>-0.99349144049751503</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -574,10 +574,10 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>52.355518000000004</v>
+        <v>52.219977</v>
       </c>
       <c r="C5">
-        <v>-1.17432</v>
+        <v>0.48757800000000001</v>
       </c>
       <c r="D5">
         <v>25</v>
@@ -588,10 +588,10 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>52.825868</v>
+        <v>52.451239999999999</v>
       </c>
       <c r="C6">
-        <v>-1.3310310000000001</v>
+        <v>-1.937937</v>
       </c>
       <c r="D6">
         <v>59</v>
@@ -602,10 +602,10 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>52.019029000000003</v>
+        <v>54.068092449999902</v>
       </c>
       <c r="C7">
-        <v>-0.77042699999999997</v>
+        <v>-2.6852531259442101</v>
       </c>
       <c r="D7">
         <v>77</v>
@@ -616,10 +616,10 @@
         <v>4</v>
       </c>
       <c r="B8">
-        <v>55.953251000000002</v>
+        <v>56.786111200000001</v>
       </c>
       <c r="C8">
-        <v>-3.1882670000000002</v>
+        <v>-4.1140518000000004</v>
       </c>
       <c r="D8">
         <v>84</v>
@@ -630,10 +630,10 @@
         <v>5</v>
       </c>
       <c r="B9">
-        <v>51.481583000000001</v>
+        <v>52.2928116</v>
       </c>
       <c r="C9">
-        <v>-3.17909</v>
+        <v>-3.7389299999999999</v>
       </c>
       <c r="D9">
         <v>99</v>
@@ -644,10 +644,10 @@
         <v>6</v>
       </c>
       <c r="B10">
-        <v>54.787714999999999</v>
+        <v>54.585983599999999</v>
       </c>
       <c r="C10">
-        <v>-6.4923149999999996</v>
+        <v>-6.9591554000000002</v>
       </c>
       <c r="D10">
         <v>2</v>

</xml_diff>